<commit_message>
Rohith - Commit - August 15th, 12:21 AM
</commit_message>
<xml_diff>
--- a/POM/data/TC003.xlsx
+++ b/POM/data/TC003.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Username</t>
   </si>
@@ -24,6 +24,9 @@
     <t>crmsfa</t>
   </si>
   <si>
+    <t>DemoCSR</t>
+  </si>
+  <si>
     <t>Password</t>
   </si>
   <si>
@@ -39,13 +42,22 @@
     <t>DemoSalesManager</t>
   </si>
   <si>
-    <t>CTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rohith </t>
-  </si>
-  <si>
-    <t>Nandakumar</t>
+    <t>SalesForce</t>
+  </si>
+  <si>
+    <t>Paypal</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Hendrix</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>Paul</t>
   </si>
 </sst>
 </file>
@@ -384,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -395,7 +407,8 @@
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -403,33 +416,50 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>